<commit_message>
add auto remove function & refine the structure for the xlsx input
</commit_message>
<xml_diff>
--- a/autogen_sentence/爆款文案_2024.xlsx
+++ b/autogen_sentence/爆款文案_2024.xlsx
@@ -29,9 +29,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
-  <si>
-    <t>需要批量产生的条数:</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+  <si>
+    <t>需要批量产生的句条数:</t>
+  </si>
+  <si>
+    <t>需要批量产生的文案条数:</t>
   </si>
   <si>
     <t>序号</t>
@@ -1654,12 +1657,12 @@
   <dimension ref="A2:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="1" max="1" width="25.3333333333333" customWidth="1"/>
     <col min="2" max="2" width="81.4444444444444" customWidth="1"/>
     <col min="3" max="3" width="14.7777777777778" customWidth="1"/>
   </cols>
@@ -1673,8 +1676,12 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>10000</v>
+      </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5"/>
@@ -1698,10 +1705,10 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" ht="114" customHeight="1" spans="1:2">
@@ -1709,7 +1716,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" ht="43.2" spans="1:2">
@@ -1717,7 +1724,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1743,277 +1750,277 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>